<commit_message>
data filled in dashborad child name, number of tests
</commit_message>
<xml_diff>
--- a/xlsautomation/NoteRating.xlsx
+++ b/xlsautomation/NoteRating.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -46,13 +46,21 @@
       <family val="0"/>
       <sz val="14"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCC99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,7 +82,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -87,6 +95,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -465,14 +474,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>#of tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anika</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Adithya</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ananya</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -486,316 +538,316 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="19.04" customWidth="1" style="4" min="1" max="1"/>
-    <col width="17.09" customWidth="1" style="4" min="2" max="2"/>
-    <col width="15" customWidth="1" style="4" min="3" max="3"/>
-    <col width="16.53" customWidth="1" style="4" min="4" max="4"/>
-    <col width="15.28" customWidth="1" style="4" min="5" max="5"/>
-    <col width="13.89" customWidth="1" style="4" min="6" max="6"/>
-    <col width="11.52" customWidth="1" style="4" min="7" max="1025"/>
+    <col width="19.04" customWidth="1" style="5" min="1" max="1"/>
+    <col width="17.09" customWidth="1" style="5" min="2" max="2"/>
+    <col width="15" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.53" customWidth="1" style="5" min="4" max="4"/>
+    <col width="15.28" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.89" customWidth="1" style="5" min="6" max="6"/>
+    <col width="11.52" customWidth="1" style="5" min="7" max="1025"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Examtype</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Marksgot</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>TotalMarks</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A2" s="5" t="inlineStr">
+    <row r="2" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Anika</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>22.5</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A3" s="5" t="inlineStr">
+    <row r="3" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Adithya</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="7" t="n">
         <v>18.5</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="7" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A4" s="5" t="inlineStr">
+    <row r="4" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Ananya</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="7" t="n">
         <v>23.5</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A5" s="5" t="inlineStr">
+    <row r="5" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Anika</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Maths</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>4.5</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A6" s="5" t="inlineStr">
+    <row r="6" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Adithya</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Maths</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="7" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A7" s="5" t="inlineStr">
+    <row r="7" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Ananya</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Maths</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="7" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A8" s="5" t="inlineStr">
+    <row r="8" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Anika</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Maths</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>SA</t>
         </is>
       </c>
-      <c r="D8" s="6" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr">
         <is>
           <t>22.5</t>
         </is>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A9" s="5" t="inlineStr">
+    <row r="9" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Adithya</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Maths</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>SA</t>
         </is>
       </c>
-      <c r="D9" s="6" t="inlineStr">
+      <c r="D9" s="7" t="inlineStr">
         <is>
           <t>21.5</t>
         </is>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="17.35" customFormat="1" customHeight="1" s="5">
-      <c r="A10" s="5" t="inlineStr">
+    <row r="10" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Ananya</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Maths</t>
         </is>
       </c>
-      <c r="C10" s="5" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>SA</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr">
+      <c r="D10" s="7" t="inlineStr">
         <is>
           <t>21.5</t>
         </is>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="12" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="13" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="14" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="15" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="16" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="17" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="18" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="19" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="20" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="21" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="22" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="23" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="24" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="25" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="26" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="27" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="28" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="29" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="30" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="31" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="32" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="33" ht="17.35" customFormat="1" customHeight="1" s="5"/>
-    <row r="34" ht="17.35" customFormat="1" customHeight="1" s="5"/>
+    <row r="11" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="12" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="13" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="14" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="15" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="16" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="17" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="18" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="19" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="20" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="21" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="22" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="23" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="24" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="25" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="26" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="27" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="28" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="29" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="30" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="31" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="32" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="33" ht="17.35" customFormat="1" customHeight="1" s="6"/>
+    <row r="34" ht="17.35" customFormat="1" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>